<commit_message>
Integration extension EU bdc682306ff7e8383836c469b263c68e9208188f
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/StructureDefinition-fr-inpatient-medicationrequest.xlsx
+++ b/VoitureBalaisDecisions/ig/StructureDefinition-fr-inpatient-medicationrequest.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-12T15:19:17+00:00</t>
+    <t>2025-08-12T15:54:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -456,6 +456,26 @@
 ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
+    <t>MedicationRequest.extension:renderedDosageInstruction</t>
+  </si>
+  <si>
+    <t>renderedDosageInstruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://hl7.org/fhir/5.0/StructureDefinition/extension-MedicationRequest.renderedDosageInstruction}
+</t>
+  </si>
+  <si>
+    <t>Full representation of the dosage instructions</t>
+  </si>
+  <si>
+    <t>Optional Extension Element - found in all resources.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
     <t>MedicationRequest.extension:treatmentIntent</t>
   </si>
   <si>
@@ -472,10 +492,6 @@
     <t>the overall intention of the treatment</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
     <t>MedicationRequest.extension:treatmentIntent.id</t>
   </si>
   <si>
@@ -643,22 +659,6 @@
   </si>
   <si>
     <t>C*E.9. But note many systems use C*E.2 for this</t>
-  </si>
-  <si>
-    <t>MedicationRequest.extension:posologieTextuelle</t>
-  </si>
-  <si>
-    <t>posologieTextuelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://hl7.fr/ig/fhir/medication/StructureDefinition/eu-rendered-instruction}
-</t>
-  </si>
-  <si>
-    <t>European extension for renderedDosageInstruction</t>
-  </si>
-  <si>
-    <t>Equivalent to FHIR R5 MedicationRequest.renderedDosageInstruction</t>
   </si>
   <si>
     <t>MedicationRequest.modifierExtension</t>
@@ -4483,7 +4483,7 @@
         <v>81</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="AN10" t="s" s="2">
         <v>81</v>
@@ -4497,9 +4497,11 @@
         <v>148</v>
       </c>
       <c r="B11" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="C11" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="C11" s="2"/>
       <c r="D11" t="s" s="2">
         <v>81</v>
       </c>
@@ -4577,19 +4579,19 @@
         <v>81</v>
       </c>
       <c r="AF11" t="s" s="2">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="AG11" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>81</v>
@@ -4598,7 +4600,7 @@
         <v>81</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>154</v>
+        <v>81</v>
       </c>
       <c r="AN11" t="s" s="2">
         <v>81</v>
@@ -4609,10 +4611,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s" s="2">
@@ -4623,7 +4625,7 @@
         <v>79</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="H12" t="s" s="2">
         <v>81</v>
@@ -4635,13 +4637,13 @@
         <v>81</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
@@ -4680,16 +4682,16 @@
         <v>81</v>
       </c>
       <c r="AB12" t="s" s="2">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="AC12" t="s" s="2">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="AD12" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>158</v>
@@ -4698,13 +4700,13 @@
         <v>79</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI12" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>81</v>
@@ -4713,7 +4715,7 @@
         <v>81</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="AN12" t="s" s="2">
         <v>81</v>
@@ -4724,10 +4726,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -4735,10 +4737,10 @@
       </c>
       <c r="E13" s="2"/>
       <c r="F13" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H13" t="s" s="2">
         <v>81</v>
@@ -4750,24 +4752,22 @@
         <v>81</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>162</v>
-      </c>
-      <c r="N13" t="s" s="2">
-        <v>163</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" t="s" s="2">
         <v>81</v>
       </c>
       <c r="Q13" s="2"/>
       <c r="R13" t="s" s="2">
-        <v>164</v>
+        <v>81</v>
       </c>
       <c r="S13" t="s" s="2">
         <v>81</v>
@@ -4797,31 +4797,31 @@
         <v>81</v>
       </c>
       <c r="AB13" t="s" s="2">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="AC13" t="s" s="2">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="AD13" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AG13" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI13" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>81</v>
+        <v>141</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>81</v>
@@ -4830,7 +4830,7 @@
         <v>81</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>81</v>
@@ -4841,50 +4841,50 @@
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="E14" t="s" s="2">
+      <c r="E14" s="2"/>
+      <c r="F14" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="G14" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="H14" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="I14" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="J14" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="K14" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="L14" t="s" s="2">
+        <v>166</v>
+      </c>
+      <c r="M14" t="s" s="2">
+        <v>167</v>
+      </c>
+      <c r="N14" t="s" s="2">
         <v>168</v>
       </c>
-      <c r="F14" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="G14" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="H14" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="I14" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="J14" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="K14" t="s" s="2">
-        <v>169</v>
-      </c>
-      <c r="L14" t="s" s="2">
-        <v>170</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" t="s" s="2">
         <v>81</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" t="s" s="2">
-        <v>81</v>
+        <v>169</v>
       </c>
       <c r="S14" t="s" s="2">
         <v>81</v>
@@ -4902,13 +4902,13 @@
         <v>81</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>172</v>
+        <v>81</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="Z14" t="s" s="2">
-        <v>174</v>
+        <v>81</v>
       </c>
       <c r="AA14" t="s" s="2">
         <v>81</v>
@@ -4926,10 +4926,10 @@
         <v>81</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH14" t="s" s="2">
         <v>90</v>
@@ -4938,7 +4938,7 @@
         <v>81</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>81</v>
@@ -4958,16 +4958,18 @@
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
         <v>81</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" t="s" s="2">
+        <v>173</v>
+      </c>
       <c r="F15" t="s" s="2">
         <v>79</v>
       </c>
@@ -4984,13 +4986,13 @@
         <v>81</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>150</v>
+        <v>174</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>151</v>
+        <v>175</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -5017,13 +5019,13 @@
         <v>81</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>81</v>
@@ -5041,7 +5043,7 @@
         <v>81</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>79</v>
@@ -5053,7 +5055,7 @@
         <v>81</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>81</v>
@@ -5062,7 +5064,7 @@
         <v>81</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="AN15" t="s" s="2">
         <v>81</v>
@@ -5073,21 +5075,21 @@
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
-        <v>180</v>
+        <v>81</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>81</v>
@@ -5099,17 +5101,15 @@
         <v>81</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>182</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>183</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="N16" s="2"/>
       <c r="O16" s="2"/>
       <c r="P16" t="s" s="2">
         <v>81</v>
@@ -5146,16 +5146,16 @@
         <v>81</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="AC16" t="s" s="2">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="AD16" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>139</v>
+        <v>81</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>158</v>
@@ -5164,13 +5164,13 @@
         <v>79</v>
       </c>
       <c r="AH16" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI16" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>141</v>
+        <v>81</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>81</v>
@@ -5179,7 +5179,7 @@
         <v>81</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN16" t="s" s="2">
         <v>81</v>
@@ -5190,14 +5190,14 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
+        <v>183</v>
+      </c>
+      <c r="B17" t="s" s="2">
         <v>184</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>185</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" t="s" s="2">
@@ -5213,23 +5213,21 @@
         <v>81</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="K17" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>187</v>
       </c>
-      <c r="M17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>188</v>
       </c>
-      <c r="N17" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="O17" t="s" s="2">
-        <v>190</v>
-      </c>
+      <c r="O17" s="2"/>
       <c r="P17" t="s" s="2">
         <v>81</v>
       </c>
@@ -5265,19 +5263,19 @@
         <v>81</v>
       </c>
       <c r="AB17" t="s" s="2">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="AC17" t="s" s="2">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="AD17" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>79</v>
@@ -5289,7 +5287,7 @@
         <v>81</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>81</v>
@@ -5298,21 +5296,21 @@
         <v>81</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="AN17" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>193</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -5323,7 +5321,7 @@
         <v>79</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>81</v>
@@ -5335,19 +5333,19 @@
         <v>91</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="O18" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="P18" t="s" s="2">
         <v>81</v>
@@ -5396,13 +5394,13 @@
         <v>81</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH18" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI18" t="s" s="2">
         <v>81</v>
@@ -5417,25 +5415,23 @@
         <v>81</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="AN18" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="C19" t="s" s="2">
-        <v>204</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
         <v>81</v>
       </c>
@@ -5453,19 +5449,23 @@
         <v>81</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+        <v>202</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="O19" t="s" s="2">
+        <v>204</v>
+      </c>
       <c r="P19" t="s" s="2">
         <v>81</v>
       </c>
@@ -5513,19 +5513,19 @@
         <v>81</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>140</v>
+        <v>205</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH19" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI19" t="s" s="2">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>141</v>
+        <v>102</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>81</v>
@@ -5534,13 +5534,13 @@
         <v>81</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="AN19" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO19" t="s" s="2">
-        <v>81</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20">
@@ -5552,7 +5552,7 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
@@ -5580,7 +5580,7 @@
         <v>210</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>211</v>
@@ -5924,7 +5924,7 @@
         <v>81</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L23" t="s" s="2">
         <v>235</v>
@@ -6158,7 +6158,7 @@
         <v>81</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L25" t="s" s="2">
         <v>253</v>
@@ -6856,13 +6856,13 @@
         <v>81</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" s="2"/>
@@ -6913,7 +6913,7 @@
         <v>81</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -6934,7 +6934,7 @@
         <v>81</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>81</v>
@@ -6952,7 +6952,7 @@
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" t="s" s="2">
@@ -6974,13 +6974,13 @@
         <v>135</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
@@ -7021,7 +7021,7 @@
         <v>138</v>
       </c>
       <c r="AC32" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD32" t="s" s="2">
         <v>81</v>
@@ -7030,7 +7030,7 @@
         <v>139</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
@@ -7051,7 +7051,7 @@
         <v>81</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>81</v>
@@ -7147,7 +7147,7 @@
         <v>81</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>79</v>
@@ -7205,7 +7205,7 @@
         <v>91</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L34" t="s" s="2">
         <v>307</v>
@@ -7357,7 +7357,7 @@
         <v>81</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="Y35" t="s" s="2">
         <v>317</v>
@@ -7556,7 +7556,7 @@
         <v>91</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L37" t="s" s="2">
         <v>329</v>
@@ -7675,7 +7675,7 @@
         <v>91</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L38" t="s" s="2">
         <v>281</v>
@@ -7790,13 +7790,13 @@
         <v>81</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -7847,7 +7847,7 @@
         <v>81</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -7868,7 +7868,7 @@
         <v>81</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>81</v>
@@ -7886,7 +7886,7 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -7908,13 +7908,13 @@
         <v>135</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
@@ -7955,7 +7955,7 @@
         <v>138</v>
       </c>
       <c r="AC40" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD40" t="s" s="2">
         <v>81</v>
@@ -7964,7 +7964,7 @@
         <v>139</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -7985,7 +7985,7 @@
         <v>81</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>81</v>
@@ -8081,7 +8081,7 @@
         <v>81</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -8139,19 +8139,19 @@
         <v>91</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="M42" t="s" s="2">
         <v>341</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>81</v>
@@ -8200,7 +8200,7 @@
         <v>81</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -8221,13 +8221,13 @@
         <v>81</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43">
@@ -8258,19 +8258,19 @@
         <v>91</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="O43" t="s" s="2">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>81</v>
@@ -8319,7 +8319,7 @@
         <v>81</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -8340,13 +8340,13 @@
         <v>81</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="44">
@@ -8726,13 +8726,13 @@
         <v>81</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -8783,7 +8783,7 @@
         <v>81</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -8804,7 +8804,7 @@
         <v>81</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>81</v>
@@ -8822,7 +8822,7 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
@@ -8844,13 +8844,13 @@
         <v>135</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O48" s="2"/>
       <c r="P48" t="s" s="2">
@@ -8891,7 +8891,7 @@
         <v>138</v>
       </c>
       <c r="AC48" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD48" t="s" s="2">
         <v>81</v>
@@ -8900,7 +8900,7 @@
         <v>139</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -8921,7 +8921,7 @@
         <v>81</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>81</v>
@@ -9017,7 +9017,7 @@
         <v>81</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -9075,7 +9075,7 @@
         <v>91</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L50" t="s" s="2">
         <v>307</v>
@@ -9227,7 +9227,7 @@
         <v>81</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="Y51" t="s" s="2">
         <v>317</v>
@@ -9426,7 +9426,7 @@
         <v>91</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>329</v>
@@ -9888,7 +9888,7 @@
         <v>91</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L57" t="s" s="2">
         <v>403</v>
@@ -10120,7 +10120,7 @@
         <v>81</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L59" t="s" s="2">
         <v>417</v>
@@ -10816,7 +10816,7 @@
         <v>81</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L65" t="s" s="2">
         <v>456</v>
@@ -11163,13 +11163,13 @@
         <v>81</v>
       </c>
       <c r="K68" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -11220,7 +11220,7 @@
         <v>81</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>79</v>
@@ -11241,7 +11241,7 @@
         <v>81</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>81</v>
@@ -11259,7 +11259,7 @@
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E69" s="2"/>
       <c r="F69" t="s" s="2">
@@ -11281,13 +11281,13 @@
         <v>135</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N69" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O69" s="2"/>
       <c r="P69" t="s" s="2">
@@ -11328,7 +11328,7 @@
         <v>138</v>
       </c>
       <c r="AC69" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD69" t="s" s="2">
         <v>81</v>
@@ -11337,7 +11337,7 @@
         <v>139</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>79</v>
@@ -11358,7 +11358,7 @@
         <v>81</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>81</v>
@@ -11456,7 +11456,7 @@
         <v>81</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>79</v>
@@ -11978,13 +11978,13 @@
         <v>81</v>
       </c>
       <c r="K75" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -12035,7 +12035,7 @@
         <v>81</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>79</v>
@@ -12056,7 +12056,7 @@
         <v>81</v>
       </c>
       <c r="AM75" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN75" t="s" s="2">
         <v>81</v>
@@ -12074,7 +12074,7 @@
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
@@ -12096,13 +12096,13 @@
         <v>135</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N76" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O76" s="2"/>
       <c r="P76" t="s" s="2">
@@ -12143,7 +12143,7 @@
         <v>138</v>
       </c>
       <c r="AC76" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD76" t="s" s="2">
         <v>81</v>
@@ -12152,7 +12152,7 @@
         <v>139</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>79</v>
@@ -12173,7 +12173,7 @@
         <v>81</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>81</v>
@@ -12219,7 +12219,7 @@
         <v>513</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>211</v>
@@ -12446,7 +12446,7 @@
         <v>91</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L79" t="s" s="2">
         <v>524</v>
@@ -12563,7 +12563,7 @@
         <v>91</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L80" t="s" s="2">
         <v>530</v>
@@ -12682,7 +12682,7 @@
         <v>91</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L81" t="s" s="2">
         <v>539</v>
@@ -12916,13 +12916,13 @@
         <v>81</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -12973,7 +12973,7 @@
         <v>81</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>79</v>
@@ -12994,7 +12994,7 @@
         <v>81</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>81</v>
@@ -13012,7 +13012,7 @@
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -13034,13 +13034,13 @@
         <v>135</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
@@ -13081,7 +13081,7 @@
         <v>138</v>
       </c>
       <c r="AC84" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD84" t="s" s="2">
         <v>81</v>
@@ -13090,7 +13090,7 @@
         <v>139</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>79</v>
@@ -13111,7 +13111,7 @@
         <v>81</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>81</v>
@@ -13157,7 +13157,7 @@
         <v>513</v>
       </c>
       <c r="N85" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O85" t="s" s="2">
         <v>211</v>
@@ -13501,13 +13501,13 @@
         <v>81</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -13558,7 +13558,7 @@
         <v>81</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>79</v>
@@ -13579,7 +13579,7 @@
         <v>81</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN88" t="s" s="2">
         <v>81</v>
@@ -13597,7 +13597,7 @@
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E89" s="2"/>
       <c r="F89" t="s" s="2">
@@ -13619,13 +13619,13 @@
         <v>135</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N89" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
@@ -13666,7 +13666,7 @@
         <v>138</v>
       </c>
       <c r="AC89" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD89" t="s" s="2">
         <v>81</v>
@@ -13675,7 +13675,7 @@
         <v>139</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>79</v>
@@ -13696,7 +13696,7 @@
         <v>81</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>81</v>
@@ -13792,7 +13792,7 @@
         <v>81</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>79</v>
@@ -15207,7 +15207,7 @@
         <v>81</v>
       </c>
       <c r="AM102" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN102" t="s" s="2">
         <v>81</v>
@@ -15324,7 +15324,7 @@
         <v>81</v>
       </c>
       <c r="AM103" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN103" t="s" s="2">
         <v>81</v>
@@ -15595,7 +15595,7 @@
         <v>91</v>
       </c>
       <c r="K106" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L106" t="s" s="2">
         <v>658</v>
@@ -15829,7 +15829,7 @@
         <v>91</v>
       </c>
       <c r="K108" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L108" t="s" s="2">
         <v>676</v>
@@ -15948,7 +15948,7 @@
         <v>91</v>
       </c>
       <c r="K109" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L109" t="s" s="2">
         <v>686</v>
@@ -15983,7 +15983,7 @@
         <v>81</v>
       </c>
       <c r="X109" t="s" s="2">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="Y109" s="2"/>
       <c r="Z109" t="s" s="2">
@@ -16063,7 +16063,7 @@
         <v>91</v>
       </c>
       <c r="K110" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L110" t="s" s="2">
         <v>694</v>
@@ -16100,7 +16100,7 @@
         <v>81</v>
       </c>
       <c r="X110" t="s" s="2">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="Y110" s="2"/>
       <c r="Z110" t="s" s="2">
@@ -16295,13 +16295,13 @@
         <v>81</v>
       </c>
       <c r="K112" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L112" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M112" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N112" s="2"/>
       <c r="O112" s="2"/>
@@ -16352,7 +16352,7 @@
         <v>81</v>
       </c>
       <c r="AF112" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG112" t="s" s="2">
         <v>79</v>
@@ -16373,7 +16373,7 @@
         <v>81</v>
       </c>
       <c r="AM112" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN112" t="s" s="2">
         <v>81</v>
@@ -16391,7 +16391,7 @@
       </c>
       <c r="C113" s="2"/>
       <c r="D113" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E113" s="2"/>
       <c r="F113" t="s" s="2">
@@ -16413,13 +16413,13 @@
         <v>135</v>
       </c>
       <c r="L113" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M113" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N113" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O113" s="2"/>
       <c r="P113" t="s" s="2">
@@ -16460,7 +16460,7 @@
         <v>138</v>
       </c>
       <c r="AC113" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD113" t="s" s="2">
         <v>81</v>
@@ -16469,7 +16469,7 @@
         <v>139</v>
       </c>
       <c r="AF113" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG113" t="s" s="2">
         <v>79</v>
@@ -16490,7 +16490,7 @@
         <v>81</v>
       </c>
       <c r="AM113" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN113" t="s" s="2">
         <v>81</v>
@@ -16586,7 +16586,7 @@
         <v>81</v>
       </c>
       <c r="AF114" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG114" t="s" s="2">
         <v>79</v>
@@ -16644,7 +16644,7 @@
         <v>91</v>
       </c>
       <c r="K115" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L115" t="s" s="2">
         <v>715</v>
@@ -17719,13 +17719,13 @@
         <v>81</v>
       </c>
       <c r="K124" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L124" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M124" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N124" s="2"/>
       <c r="O124" s="2"/>
@@ -17776,7 +17776,7 @@
         <v>81</v>
       </c>
       <c r="AF124" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG124" t="s" s="2">
         <v>79</v>
@@ -17797,7 +17797,7 @@
         <v>81</v>
       </c>
       <c r="AM124" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN124" t="s" s="2">
         <v>81</v>
@@ -17815,7 +17815,7 @@
       </c>
       <c r="C125" s="2"/>
       <c r="D125" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E125" s="2"/>
       <c r="F125" t="s" s="2">
@@ -17837,13 +17837,13 @@
         <v>135</v>
       </c>
       <c r="L125" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M125" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N125" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O125" s="2"/>
       <c r="P125" t="s" s="2">
@@ -17884,7 +17884,7 @@
         <v>138</v>
       </c>
       <c r="AC125" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD125" t="s" s="2">
         <v>81</v>
@@ -17893,7 +17893,7 @@
         <v>139</v>
       </c>
       <c r="AF125" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG125" t="s" s="2">
         <v>79</v>
@@ -17914,7 +17914,7 @@
         <v>81</v>
       </c>
       <c r="AM125" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN125" t="s" s="2">
         <v>81</v>
@@ -18532,13 +18532,13 @@
         <v>81</v>
       </c>
       <c r="K131" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L131" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M131" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N131" s="2"/>
       <c r="O131" s="2"/>
@@ -18589,7 +18589,7 @@
         <v>81</v>
       </c>
       <c r="AF131" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG131" t="s" s="2">
         <v>79</v>
@@ -18610,7 +18610,7 @@
         <v>81</v>
       </c>
       <c r="AM131" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN131" t="s" s="2">
         <v>81</v>
@@ -18628,7 +18628,7 @@
       </c>
       <c r="C132" s="2"/>
       <c r="D132" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E132" s="2"/>
       <c r="F132" t="s" s="2">
@@ -18650,13 +18650,13 @@
         <v>135</v>
       </c>
       <c r="L132" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M132" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N132" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O132" s="2"/>
       <c r="P132" t="s" s="2">
@@ -18706,7 +18706,7 @@
         <v>81</v>
       </c>
       <c r="AF132" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG132" t="s" s="2">
         <v>79</v>
@@ -18727,7 +18727,7 @@
         <v>81</v>
       </c>
       <c r="AM132" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN132" t="s" s="2">
         <v>81</v>
@@ -18773,7 +18773,7 @@
         <v>513</v>
       </c>
       <c r="N133" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O133" t="s" s="2">
         <v>211</v>
@@ -19000,13 +19000,13 @@
         <v>81</v>
       </c>
       <c r="K135" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L135" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M135" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N135" s="2"/>
       <c r="O135" s="2"/>
@@ -19057,7 +19057,7 @@
         <v>81</v>
       </c>
       <c r="AF135" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG135" t="s" s="2">
         <v>79</v>
@@ -19078,7 +19078,7 @@
         <v>81</v>
       </c>
       <c r="AM135" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN135" t="s" s="2">
         <v>81</v>
@@ -19096,7 +19096,7 @@
       </c>
       <c r="C136" s="2"/>
       <c r="D136" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E136" s="2"/>
       <c r="F136" t="s" s="2">
@@ -19118,13 +19118,13 @@
         <v>135</v>
       </c>
       <c r="L136" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M136" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N136" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O136" s="2"/>
       <c r="P136" t="s" s="2">
@@ -19174,7 +19174,7 @@
         <v>81</v>
       </c>
       <c r="AF136" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG136" t="s" s="2">
         <v>79</v>
@@ -19195,7 +19195,7 @@
         <v>81</v>
       </c>
       <c r="AM136" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN136" t="s" s="2">
         <v>81</v>
@@ -19241,7 +19241,7 @@
         <v>513</v>
       </c>
       <c r="N137" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O137" t="s" s="2">
         <v>211</v>
@@ -19815,13 +19815,13 @@
         <v>81</v>
       </c>
       <c r="K142" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L142" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M142" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N142" s="2"/>
       <c r="O142" s="2"/>
@@ -19872,7 +19872,7 @@
         <v>81</v>
       </c>
       <c r="AF142" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG142" t="s" s="2">
         <v>79</v>
@@ -19893,7 +19893,7 @@
         <v>81</v>
       </c>
       <c r="AM142" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN142" t="s" s="2">
         <v>81</v>
@@ -19911,7 +19911,7 @@
       </c>
       <c r="C143" s="2"/>
       <c r="D143" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E143" s="2"/>
       <c r="F143" t="s" s="2">
@@ -19933,13 +19933,13 @@
         <v>135</v>
       </c>
       <c r="L143" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M143" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N143" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O143" s="2"/>
       <c r="P143" t="s" s="2">
@@ -19980,7 +19980,7 @@
         <v>138</v>
       </c>
       <c r="AC143" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD143" t="s" s="2">
         <v>81</v>
@@ -19989,7 +19989,7 @@
         <v>139</v>
       </c>
       <c r="AF143" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG143" t="s" s="2">
         <v>79</v>
@@ -20010,7 +20010,7 @@
         <v>81</v>
       </c>
       <c r="AM143" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN143" t="s" s="2">
         <v>81</v>
@@ -20632,13 +20632,13 @@
         <v>81</v>
       </c>
       <c r="K149" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L149" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M149" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N149" s="2"/>
       <c r="O149" s="2"/>
@@ -20689,7 +20689,7 @@
         <v>81</v>
       </c>
       <c r="AF149" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG149" t="s" s="2">
         <v>79</v>
@@ -20710,7 +20710,7 @@
         <v>81</v>
       </c>
       <c r="AM149" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN149" t="s" s="2">
         <v>81</v>
@@ -20728,7 +20728,7 @@
       </c>
       <c r="C150" s="2"/>
       <c r="D150" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E150" s="2"/>
       <c r="F150" t="s" s="2">
@@ -20750,13 +20750,13 @@
         <v>135</v>
       </c>
       <c r="L150" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M150" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N150" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O150" s="2"/>
       <c r="P150" t="s" s="2">
@@ -20797,7 +20797,7 @@
         <v>138</v>
       </c>
       <c r="AC150" t="s" s="2">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="AD150" t="s" s="2">
         <v>81</v>
@@ -20806,7 +20806,7 @@
         <v>139</v>
       </c>
       <c r="AF150" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG150" t="s" s="2">
         <v>79</v>
@@ -20827,7 +20827,7 @@
         <v>81</v>
       </c>
       <c r="AM150" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN150" t="s" s="2">
         <v>81</v>
@@ -21102,7 +21102,7 @@
         <v>91</v>
       </c>
       <c r="K153" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L153" t="s" s="2">
         <v>882</v>
@@ -21685,13 +21685,13 @@
         <v>81</v>
       </c>
       <c r="K158" t="s" s="2">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="L158" t="s" s="2">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="M158" t="s" s="2">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="N158" s="2"/>
       <c r="O158" s="2"/>
@@ -21742,7 +21742,7 @@
         <v>81</v>
       </c>
       <c r="AF158" t="s" s="2">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AG158" t="s" s="2">
         <v>79</v>
@@ -21763,7 +21763,7 @@
         <v>81</v>
       </c>
       <c r="AM158" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN158" t="s" s="2">
         <v>81</v>
@@ -21781,7 +21781,7 @@
       </c>
       <c r="C159" s="2"/>
       <c r="D159" t="s" s="2">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="E159" s="2"/>
       <c r="F159" t="s" s="2">
@@ -21803,13 +21803,13 @@
         <v>135</v>
       </c>
       <c r="L159" t="s" s="2">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="M159" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="N159" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O159" s="2"/>
       <c r="P159" t="s" s="2">
@@ -21859,7 +21859,7 @@
         <v>81</v>
       </c>
       <c r="AF159" t="s" s="2">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="AG159" t="s" s="2">
         <v>79</v>
@@ -21880,7 +21880,7 @@
         <v>81</v>
       </c>
       <c r="AM159" t="s" s="2">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AN159" t="s" s="2">
         <v>81</v>
@@ -21926,7 +21926,7 @@
         <v>513</v>
       </c>
       <c r="N160" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="O160" t="s" s="2">
         <v>211</v>
@@ -22153,7 +22153,7 @@
         <v>81</v>
       </c>
       <c r="K162" t="s" s="2">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="L162" t="s" s="2">
         <v>924</v>

</xml_diff>

<commit_message>
correction coquille bis 430714ffe7f2be0446e2e0212dfa79b9ca42cd07
</commit_message>
<xml_diff>
--- a/VoitureBalaisDecisions/ig/StructureDefinition-fr-inpatient-medicationrequest.xlsx
+++ b/VoitureBalaisDecisions/ig/StructureDefinition-fr-inpatient-medicationrequest.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-19T08:39:15+00:00</t>
+    <t>2025-08-19T16:40:37+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -11190,7 +11190,7 @@
         <v>79</v>
       </c>
       <c r="G69" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="H69" t="s" s="2">
         <v>81</v>

</xml_diff>